<commit_message>
data retrieval in usermode and frontend updates
</commit_message>
<xml_diff>
--- a/Audit_Output.xlsx
+++ b/Audit_Output.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -465,10 +465,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -477,10 +477,12 @@
     <col width="43.6640625" customWidth="1" min="2" max="2"/>
     <col width="47" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="42.33203125" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="29" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="6" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="4.88671875" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="9" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="42.33203125" customWidth="1" min="5" max="5"/>
+    <col width="29" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="29" customWidth="1" min="7" max="11"/>
+    <col width="6" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="4.88671875" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="9" bestFit="1" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="5">
@@ -506,20 +508,50 @@
       </c>
       <c r="E1" s="4" t="inlineStr">
         <is>
+          <t>owner</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
           <t>Assigne</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>checked out to</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>hs-code</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>purchase cost</t>
+        </is>
+      </c>
+      <c r="L1" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="M1" s="5" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="N1" s="5" t="inlineStr">
         <is>
           <t>Comment</t>
         </is>
@@ -540,16 +572,21 @@
           <t>Screwdriver</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Abdalla Hussein Rashad Mohamed</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>Abdalla Hussein Rashad Mohamed</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
+      <c r="J2" s="1" t="n"/>
+      <c r="K2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -566,12 +603,22 @@
           <t>3PCS Wire Brush Set</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
+      <c r="E3" s="1" t="n"/>
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>Abdalla Hussein Rashad Mohamed</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>Abdalla Hussein Rashad Mohamed</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="n"/>
+      <c r="I3" s="1" t="n"/>
+      <c r="J3" s="1" t="n"/>
+      <c r="K3" s="1" t="n"/>
+      <c r="L3" t="inlineStr">
         <is>
           <t>True</t>
         </is>
@@ -594,11 +641,21 @@
           <t>OBC AMG11</t>
         </is>
       </c>
-      <c r="E4" s="1" t="inlineStr">
+      <c r="E4" s="1" t="n"/>
+      <c r="F4" s="1" t="inlineStr">
         <is>
           <t>Abdullah Mohy</t>
         </is>
       </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>Abdalla Hussein Rashad Mohamed</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="n"/>
+      <c r="I4" s="1" t="n"/>
+      <c r="J4" s="1" t="n"/>
+      <c r="K4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -617,11 +674,21 @@
           <t>E-compressor</t>
         </is>
       </c>
-      <c r="E5" s="1" t="inlineStr">
+      <c r="E5" s="1" t="n"/>
+      <c r="F5" s="1" t="inlineStr">
         <is>
           <t>Ehab Gamal</t>
         </is>
       </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>Abdalla Hussein Rashad Mohamed</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="n"/>
+      <c r="I5" s="1" t="n"/>
+      <c r="J5" s="1" t="n"/>
+      <c r="K5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -638,16 +705,17 @@
           <t>Crimping Tool</t>
         </is>
       </c>
-      <c r="E6" s="1" t="inlineStr">
+      <c r="E6" s="1" t="n"/>
+      <c r="F6" s="1" t="inlineStr">
         <is>
           <t>Abdallah Afifi</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="G6" s="1" t="n"/>
+      <c r="H6" s="1" t="n"/>
+      <c r="I6" s="1" t="n"/>
+      <c r="J6" s="1" t="n"/>
+      <c r="K6" s="1" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -664,11 +732,17 @@
           <t>Replacement Sponge</t>
         </is>
       </c>
-      <c r="E7" s="1" t="inlineStr">
+      <c r="E7" s="1" t="n"/>
+      <c r="F7" s="1" t="inlineStr">
         <is>
           <t>Mazen Hossam ElDeen</t>
         </is>
       </c>
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="1" t="n"/>
+      <c r="I7" s="1" t="n"/>
+      <c r="J7" s="1" t="n"/>
+      <c r="K7" s="1" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -685,7 +759,13 @@
           <t>Soldering Iron Equivalent 100W</t>
         </is>
       </c>
-      <c r="E8" s="2" t="n"/>
+      <c r="E8" s="1" t="n"/>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="2" t="n"/>
+      <c r="J8" s="2" t="n"/>
+      <c r="K8" s="2" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -702,11 +782,17 @@
           <t>Screwdriver 6pcs Set</t>
         </is>
       </c>
-      <c r="E9" s="1" t="inlineStr">
+      <c r="E9" s="1" t="n"/>
+      <c r="F9" s="1" t="inlineStr">
         <is>
           <t>Mazen Hossam ElDeen</t>
         </is>
       </c>
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="1" t="n"/>
+      <c r="I9" s="1" t="n"/>
+      <c r="J9" s="1" t="n"/>
+      <c r="K9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -723,11 +809,17 @@
           <t>Knife Cutter 18mm</t>
         </is>
       </c>
-      <c r="E10" s="1" t="inlineStr">
+      <c r="E10" s="1" t="n"/>
+      <c r="F10" s="1" t="inlineStr">
         <is>
           <t>Mazen Hossam ElDeen</t>
         </is>
       </c>
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="1" t="n"/>
+      <c r="I10" s="1" t="n"/>
+      <c r="J10" s="1" t="n"/>
+      <c r="K10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -744,16 +836,17 @@
           <t>Plastic Fliptop Boxes</t>
         </is>
       </c>
-      <c r="E11" s="1" t="inlineStr">
+      <c r="E11" s="1" t="n"/>
+      <c r="F11" s="1" t="inlineStr">
         <is>
           <t>Mazen Hossam ElDeen</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="G11" s="1" t="n"/>
+      <c r="H11" s="1" t="n"/>
+      <c r="I11" s="1" t="n"/>
+      <c r="J11" s="1" t="n"/>
+      <c r="K11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -770,11 +863,17 @@
           <t>Wall Mount Power Supply</t>
         </is>
       </c>
-      <c r="E12" s="1" t="inlineStr">
+      <c r="E12" s="1" t="n"/>
+      <c r="F12" s="1" t="inlineStr">
         <is>
           <t>Abdalla Hussein Rashad Mohamed</t>
         </is>
       </c>
+      <c r="G12" s="1" t="n"/>
+      <c r="H12" s="1" t="n"/>
+      <c r="I12" s="1" t="n"/>
+      <c r="J12" s="1" t="n"/>
+      <c r="K12" s="1" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -791,11 +890,17 @@
           <t>General Purpose Probe</t>
         </is>
       </c>
-      <c r="E13" s="1" t="inlineStr">
+      <c r="E13" s="1" t="n"/>
+      <c r="F13" s="1" t="inlineStr">
         <is>
           <t>Ahmed Elbadry</t>
         </is>
       </c>
+      <c r="G13" s="1" t="n"/>
+      <c r="H13" s="1" t="n"/>
+      <c r="I13" s="1" t="n"/>
+      <c r="J13" s="1" t="n"/>
+      <c r="K13" s="1" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -816,11 +921,17 @@
           <t>Digital Oscilloscope 4 channels</t>
         </is>
       </c>
-      <c r="E14" s="1" t="inlineStr">
+      <c r="E14" s="1" t="n"/>
+      <c r="F14" s="1" t="inlineStr">
         <is>
           <t>Mohamed Hossam Eldin</t>
         </is>
       </c>
+      <c r="G14" s="1" t="n"/>
+      <c r="H14" s="1" t="n"/>
+      <c r="I14" s="1" t="n"/>
+      <c r="J14" s="1" t="n"/>
+      <c r="K14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -839,11 +950,17 @@
           <t>High Voltage Differential Probe</t>
         </is>
       </c>
-      <c r="E15" s="1" t="inlineStr">
+      <c r="E15" s="1" t="n"/>
+      <c r="F15" s="1" t="inlineStr">
         <is>
           <t>Mohamed Hossam Eldin</t>
         </is>
       </c>
+      <c r="G15" s="1" t="n"/>
+      <c r="H15" s="1" t="n"/>
+      <c r="I15" s="1" t="n"/>
+      <c r="J15" s="1" t="n"/>
+      <c r="K15" s="1" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -860,11 +977,17 @@
           <t>Cable with connector</t>
         </is>
       </c>
-      <c r="E16" s="1" t="inlineStr">
+      <c r="E16" s="1" t="n"/>
+      <c r="F16" s="1" t="inlineStr">
         <is>
           <t>Ahmed Tarek Abourady</t>
         </is>
       </c>
+      <c r="G16" s="1" t="n"/>
+      <c r="H16" s="1" t="n"/>
+      <c r="I16" s="1" t="n"/>
+      <c r="J16" s="1" t="n"/>
+      <c r="K16" s="1" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -885,16 +1008,17 @@
           <t>CANFD/LIN</t>
         </is>
       </c>
-      <c r="E17" s="1" t="inlineStr">
+      <c r="E17" s="1" t="n"/>
+      <c r="F17" s="1" t="inlineStr">
         <is>
           <t>Abdelrahman Ahmed</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="G17" s="1" t="n"/>
+      <c r="H17" s="1" t="n"/>
+      <c r="I17" s="1" t="n"/>
+      <c r="J17" s="1" t="n"/>
+      <c r="K17" s="1" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -913,12 +1037,22 @@
           <t>CAN Cable 2Y</t>
         </is>
       </c>
-      <c r="E18" s="1" t="inlineStr">
+      <c r="E18" s="1" t="n"/>
+      <c r="F18" s="1" t="inlineStr">
         <is>
           <t>Belal Sayed Ali</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" s="1" t="inlineStr">
+        <is>
+          <t>Abdalla Hussein Rashad Mohamed</t>
+        </is>
+      </c>
+      <c r="H18" s="1" t="n"/>
+      <c r="I18" s="1" t="n"/>
+      <c r="J18" s="1" t="n"/>
+      <c r="K18" s="1" t="n"/>
+      <c r="L18" t="inlineStr">
         <is>
           <t>True</t>
         </is>
@@ -945,11 +1079,17 @@
           <t>Power Supply - ZHAOXIN - 30V/10A</t>
         </is>
       </c>
-      <c r="E19" s="1" t="inlineStr">
+      <c r="E19" s="1" t="n"/>
+      <c r="F19" s="1" t="inlineStr">
         <is>
           <t>Abdelrahman Ahmed</t>
         </is>
       </c>
+      <c r="G19" s="1" t="n"/>
+      <c r="H19" s="1" t="n"/>
+      <c r="I19" s="1" t="n"/>
+      <c r="J19" s="1" t="n"/>
+      <c r="K19" s="1" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
@@ -968,11 +1108,17 @@
           <t>Hot Air Soldering Station</t>
         </is>
       </c>
-      <c r="E20" s="1" t="inlineStr">
+      <c r="E20" s="1" t="n"/>
+      <c r="F20" s="1" t="inlineStr">
         <is>
           <t>Abdelmomen Mahgoub</t>
         </is>
       </c>
+      <c r="G20" s="1" t="n"/>
+      <c r="H20" s="1" t="n"/>
+      <c r="I20" s="1" t="n"/>
+      <c r="J20" s="1" t="n"/>
+      <c r="K20" s="1" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -993,11 +1139,17 @@
           <t>Power Supply - ZHAOXIN - 30V/5A</t>
         </is>
       </c>
-      <c r="E21" s="1" t="inlineStr">
+      <c r="E21" s="1" t="n"/>
+      <c r="F21" s="1" t="inlineStr">
         <is>
           <t>George Halim</t>
         </is>
       </c>
+      <c r="G21" s="1" t="n"/>
+      <c r="H21" s="1" t="n"/>
+      <c r="I21" s="1" t="n"/>
+      <c r="J21" s="1" t="n"/>
+      <c r="K21" s="1" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -1014,11 +1166,17 @@
           <t>LIN Transceiver</t>
         </is>
       </c>
-      <c r="E22" s="1" t="inlineStr">
+      <c r="E22" s="1" t="n"/>
+      <c r="F22" s="1" t="inlineStr">
         <is>
           <t>Ahmed Adel El-Behairy</t>
         </is>
       </c>
+      <c r="G22" s="1" t="n"/>
+      <c r="H22" s="1" t="n"/>
+      <c r="I22" s="1" t="n"/>
+      <c r="J22" s="1" t="n"/>
+      <c r="K22" s="1" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1035,11 +1193,17 @@
           <t>USB to UART</t>
         </is>
       </c>
-      <c r="E23" s="1" t="inlineStr">
+      <c r="E23" s="1" t="n"/>
+      <c r="F23" s="1" t="inlineStr">
         <is>
           <t>Ahmed Adel El-Behairy</t>
         </is>
       </c>
+      <c r="G23" s="1" t="n"/>
+      <c r="H23" s="1" t="n"/>
+      <c r="I23" s="1" t="n"/>
+      <c r="J23" s="1" t="n"/>
+      <c r="K23" s="1" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -1056,12 +1220,18 @@
           <t>DB9 Female Converter</t>
         </is>
       </c>
-      <c r="E24" s="1" t="inlineStr">
+      <c r="E24" s="1" t="n"/>
+      <c r="F24" s="1" t="inlineStr">
         <is>
           <t>Esmat saied</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" s="1" t="n"/>
+      <c r="H24" s="1" t="n"/>
+      <c r="I24" s="1" t="n"/>
+      <c r="J24" s="1" t="n"/>
+      <c r="K24" s="1" t="n"/>
+      <c r="L24" t="inlineStr">
         <is>
           <t>True</t>
         </is>
@@ -1086,11 +1256,17 @@
           <t>Oil pump</t>
         </is>
       </c>
-      <c r="E25" s="1" t="inlineStr">
+      <c r="E25" s="1" t="n"/>
+      <c r="F25" s="1" t="inlineStr">
         <is>
           <t>Ahmed Saleh</t>
         </is>
       </c>
+      <c r="G25" s="1" t="n"/>
+      <c r="H25" s="1" t="n"/>
+      <c r="I25" s="1" t="n"/>
+      <c r="J25" s="1" t="n"/>
+      <c r="K25" s="1" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -1107,11 +1283,17 @@
           <t>DCABLE-AUTO26-V2 LA-3203</t>
         </is>
       </c>
-      <c r="E26" s="1" t="inlineStr">
+      <c r="E26" s="1" t="n"/>
+      <c r="F26" s="1" t="inlineStr">
         <is>
           <t>Mohamed Wahdan</t>
         </is>
       </c>
+      <c r="G26" s="1" t="n"/>
+      <c r="H26" s="1" t="n"/>
+      <c r="I26" s="1" t="n"/>
+      <c r="J26" s="1" t="n"/>
+      <c r="K26" s="1" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -1130,11 +1312,17 @@
           <t>DCABLE-AUTO26-V2 LA-3203</t>
         </is>
       </c>
-      <c r="E27" s="1" t="inlineStr">
+      <c r="E27" s="1" t="n"/>
+      <c r="F27" s="1" t="inlineStr">
         <is>
           <t>Ahmed Wageh</t>
         </is>
       </c>
+      <c r="G27" s="1" t="n"/>
+      <c r="H27" s="1" t="n"/>
+      <c r="I27" s="1" t="n"/>
+      <c r="J27" s="1" t="n"/>
+      <c r="K27" s="1" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -1155,16 +1343,17 @@
           <t>Oil pump</t>
         </is>
       </c>
-      <c r="E28" s="1" t="inlineStr">
+      <c r="E28" s="1" t="n"/>
+      <c r="F28" s="1" t="inlineStr">
         <is>
           <t>Belal Sayed Ali</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="G28" s="1" t="n"/>
+      <c r="H28" s="1" t="n"/>
+      <c r="I28" s="1" t="n"/>
+      <c r="J28" s="1" t="n"/>
+      <c r="K28" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>